<commit_message>
added output mode in DB
</commit_message>
<xml_diff>
--- a/src/main/resources/Input.xlsx
+++ b/src/main/resources/Input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Documents/_Work/code/linkedinmarketing/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{215408EA-4606-8E4F-9125-86FE60B1B1AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDFB3C53-83FB-CE40-AABD-6B6AE21AAAAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16000" activeTab="1" xr2:uid="{E270F5DC-0382-8742-A6C3-9CC777D26C2A}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16000" activeTab="5" xr2:uid="{E270F5DC-0382-8742-A6C3-9CC777D26C2A}"/>
   </bookViews>
   <sheets>
     <sheet name="raw (2)" sheetId="10" r:id="rId1"/>
@@ -76,12 +76,6 @@
     <t>name</t>
   </si>
   <si>
-    <t>sunalps2000@gmail.com</t>
-  </si>
-  <si>
-    <t>Mswinse123</t>
-  </si>
-  <si>
     <t>https://www.linkedin.com/in/mohitmalik1/</t>
   </si>
   <si>
@@ -335,6 +329,12 @@
   </si>
   <si>
     <t>https://www.linkedin.com/in/kaustuvmani-talukdar/</t>
+  </si>
+  <si>
+    <t>outputIn</t>
+  </si>
+  <si>
+    <t>DB</t>
   </si>
 </sst>
 </file>
@@ -386,7 +386,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -409,18 +409,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -764,10 +776,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -775,10 +787,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -786,10 +798,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -797,10 +809,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -808,10 +820,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -819,10 +831,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -830,10 +842,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -841,10 +853,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -852,10 +864,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -863,10 +875,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -874,10 +886,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -885,10 +897,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -896,10 +908,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -907,10 +919,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C15" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -918,10 +930,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C16" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -929,10 +941,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C17" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -940,10 +952,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C18" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -951,10 +963,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C19" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -962,10 +974,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C20" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -973,10 +985,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C21" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -984,10 +996,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C22" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -995,10 +1007,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C23" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -1006,10 +1018,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C24" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -1017,10 +1029,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C25" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -1028,10 +1040,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C26" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -1039,10 +1051,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C27" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -1050,10 +1062,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C28" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -1061,10 +1073,10 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C29" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -1072,10 +1084,10 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C30" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -1083,10 +1095,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C31" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -1094,10 +1106,10 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C32" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -1105,10 +1117,10 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C33" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -1116,10 +1128,10 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C34" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -1127,10 +1139,10 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C35" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -1138,10 +1150,10 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C36" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -1149,10 +1161,10 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C37" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -1160,10 +1172,10 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C38" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -1171,10 +1183,10 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C39" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -1182,10 +1194,10 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C40" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -1193,10 +1205,10 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C41" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -1204,10 +1216,10 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C42" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -1215,10 +1227,10 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C43" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -1226,10 +1238,10 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C44" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
@@ -1237,10 +1249,10 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C45" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
@@ -1248,10 +1260,10 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C46" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
@@ -1259,10 +1271,10 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C47" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
@@ -1270,10 +1282,10 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C48" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -1281,10 +1293,10 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C49" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -1292,10 +1304,10 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C50" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -1303,10 +1315,10 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C51" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -1314,10 +1326,10 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C52" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
@@ -1325,10 +1337,10 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C53" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
@@ -1336,10 +1348,10 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C54" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
@@ -1347,10 +1359,10 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C55" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
@@ -1358,10 +1370,10 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C56" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
@@ -1369,10 +1381,10 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C57" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
@@ -1380,10 +1392,10 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C58" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
@@ -1391,10 +1403,10 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C59" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
@@ -1402,10 +1414,10 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C60" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
@@ -1413,10 +1425,10 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C61" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
@@ -1424,10 +1436,10 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C62" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
@@ -1435,10 +1447,10 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C63" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
@@ -1446,10 +1458,10 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C64" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
@@ -1457,10 +1469,10 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C65" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
@@ -1468,10 +1480,10 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C66" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
@@ -1479,10 +1491,10 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C67" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
@@ -1490,10 +1502,10 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C68" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
@@ -1501,10 +1513,10 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C69" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
@@ -1512,10 +1524,10 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C70" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
@@ -1523,10 +1535,10 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C71" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
@@ -1534,10 +1546,10 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C72" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
@@ -1545,10 +1557,10 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C73" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
@@ -1556,10 +1568,10 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C74" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
@@ -1567,10 +1579,10 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C75" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
@@ -1578,10 +1590,10 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C76" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
@@ -1589,10 +1601,10 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C77" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
@@ -1600,10 +1612,10 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C78" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
@@ -1611,10 +1623,10 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C79" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
@@ -1622,10 +1634,10 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C80" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
@@ -1633,10 +1645,10 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C81" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1648,7 +1660,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A731CCC0-38E9-844C-8737-200721EF57F9}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -1674,10 +1686,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1685,10 +1697,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1696,10 +1708,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -1707,10 +1719,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1718,10 +1730,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -1729,10 +1741,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -1740,10 +1752,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -1751,10 +1763,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -1762,10 +1774,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1892,22 +1904,22 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1918,10 +1930,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05527DCA-48B0-0341-8236-D373F1F9225C}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1930,7 +1942,7 @@
     <col min="3" max="3" width="10.83203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -1940,27 +1952,21 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" s="6" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1" t="s">
+        <v>98</v>
+      </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{5ED28513-8E2A-454D-A3E0-477EAABD5B2F}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed issue of LinkedinSend Message
</commit_message>
<xml_diff>
--- a/src/main/resources/Input.xlsx
+++ b/src/main/resources/Input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Documents/_Work/code/linkedinmarketing/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDFB3C53-83FB-CE40-AABD-6B6AE21AAAAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A23B20EC-DFF6-8145-B701-84550762C0FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16000" activeTab="5" xr2:uid="{E270F5DC-0382-8742-A6C3-9CC777D26C2A}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="150">
   <si>
     <t>username</t>
   </si>
@@ -334,14 +334,167 @@
     <t>outputIn</t>
   </si>
   <si>
-    <t>DB</t>
+    <t>https://www.linkedin.com/in/abraham-paul-40621828/</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/gokul-menon-9a18b09b/</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/corina-pip-0949131b/</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/karishma-dambe-leader/</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/harry-long-scrum-lord/</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/narayanraman/</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/tanvi-kohli-09779414a/</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/krupa-pulijala-5b0740159/</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/meera-dileep/</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/minal-gupta/</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/vikasmittal/</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/vinothrathinamautomation/</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/narasimhan-narayanan/</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/manasju/</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/shabbirbhimani/</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/yadavmamta/</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/yatin-duggal-0885777/</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/mmronanki/</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/manoj2403/</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/sarthak-srivastava-47908565/</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/aman-srivastava-magento-dev/</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/hemanth-kumar-4b0841100/</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/andyglover-tester-leader-coach/</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/shrikantv/</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/romil-gahlaut-03304518/</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/himanshu-sharma-3928872b/</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/balaji-santhanagopalan-82a63a108/</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/jaikant-dangi/</t>
+  </si>
+  <si>
+    <t>EXCEL</t>
+  </si>
+  <si>
+    <t>Harry</t>
+  </si>
+  <si>
+    <t>2020-10-06</t>
+  </si>
+  <si>
+    <t>About |</t>
+  </si>
+  <si>
+    <t>Something went wrong</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Narayan</t>
+  </si>
+  <si>
+    <t>Krupa</t>
+  </si>
+  <si>
+    <t>Hero Image |</t>
+  </si>
+  <si>
+    <t>Minal</t>
+  </si>
+  <si>
+    <t>Vikas</t>
+  </si>
+  <si>
+    <t>Vinoth</t>
+  </si>
+  <si>
+    <t>Narasimhan</t>
+  </si>
+  <si>
+    <t>Manas</t>
+  </si>
+  <si>
+    <t>Mamta</t>
+  </si>
+  <si>
+    <t>Yatin</t>
+  </si>
+  <si>
+    <t>Madhu</t>
+  </si>
+  <si>
+    <t>Sarthak</t>
+  </si>
+  <si>
+    <t>hemanth</t>
+  </si>
+  <si>
+    <t>Andy</t>
+  </si>
+  <si>
+    <t>ShriKant</t>
+  </si>
+  <si>
+    <t>Himanshu</t>
+  </si>
+  <si>
+    <t>Balaji</t>
+  </si>
+  <si>
+    <t>Jaikant</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -370,6 +523,11 @@
       <color theme="1"/>
       <name val="Helvetica Neue"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val=".SF NS Text"/>
     </font>
   </fonts>
   <fills count="3">
@@ -425,7 +583,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -433,6 +591,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -754,13 +915,13 @@
       <selection activeCell="A2" sqref="A2:B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="2" max="2" width="56.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -771,7 +932,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -782,7 +943,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -793,7 +954,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -804,7 +965,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -815,7 +976,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -826,7 +987,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -837,7 +998,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -848,7 +1009,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -859,7 +1020,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -870,7 +1031,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -881,7 +1042,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -892,7 +1053,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -903,7 +1064,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -914,7 +1075,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -925,7 +1086,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -936,7 +1097,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -947,7 +1108,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -958,7 +1119,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -969,7 +1130,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -980,7 +1141,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -991,7 +1152,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1002,7 +1163,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1013,7 +1174,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1024,7 +1185,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1035,7 +1196,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1046,7 +1207,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1057,7 +1218,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1068,7 +1229,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1079,7 +1240,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1090,7 +1251,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1101,7 +1262,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1112,7 +1273,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1123,7 +1284,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1134,7 +1295,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1145,7 +1306,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1156,7 +1317,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1167,7 +1328,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1178,7 +1339,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1189,7 +1350,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1200,7 +1361,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1211,7 +1372,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1222,7 +1383,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1233,7 +1394,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1244,7 +1405,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1255,7 +1416,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1266,7 +1427,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1277,7 +1438,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1288,7 +1449,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1299,7 +1460,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3">
       <c r="A50">
         <v>49</v>
       </c>
@@ -1310,7 +1471,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1321,7 +1482,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3">
       <c r="A52">
         <v>51</v>
       </c>
@@ -1332,7 +1493,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3">
       <c r="A53">
         <v>52</v>
       </c>
@@ -1343,7 +1504,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3">
       <c r="A54">
         <v>53</v>
       </c>
@@ -1354,7 +1515,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3">
       <c r="A55">
         <v>54</v>
       </c>
@@ -1365,7 +1526,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3">
       <c r="A56">
         <v>55</v>
       </c>
@@ -1376,7 +1537,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3">
       <c r="A57">
         <v>56</v>
       </c>
@@ -1387,7 +1548,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3">
       <c r="A58">
         <v>57</v>
       </c>
@@ -1398,7 +1559,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3">
       <c r="A59">
         <v>58</v>
       </c>
@@ -1409,7 +1570,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3">
       <c r="A60">
         <v>59</v>
       </c>
@@ -1420,7 +1581,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:3">
       <c r="A61">
         <v>60</v>
       </c>
@@ -1431,7 +1592,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:3">
       <c r="A62">
         <v>61</v>
       </c>
@@ -1442,7 +1603,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:3">
       <c r="A63">
         <v>62</v>
       </c>
@@ -1453,7 +1614,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:3">
       <c r="A64">
         <v>63</v>
       </c>
@@ -1464,7 +1625,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:3">
       <c r="A65">
         <v>64</v>
       </c>
@@ -1475,7 +1636,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:3">
       <c r="A66">
         <v>65</v>
       </c>
@@ -1486,7 +1647,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:3">
       <c r="A67">
         <v>66</v>
       </c>
@@ -1497,7 +1658,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:3">
       <c r="A68">
         <v>67</v>
       </c>
@@ -1508,7 +1669,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:3">
       <c r="A69">
         <v>68</v>
       </c>
@@ -1519,7 +1680,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:3">
       <c r="A70">
         <v>69</v>
       </c>
@@ -1530,7 +1691,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:3">
       <c r="A71">
         <v>70</v>
       </c>
@@ -1541,7 +1702,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:3">
       <c r="A72">
         <v>71</v>
       </c>
@@ -1552,7 +1713,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:3">
       <c r="A73">
         <v>72</v>
       </c>
@@ -1563,7 +1724,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:3">
       <c r="A74">
         <v>73</v>
       </c>
@@ -1574,7 +1735,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:3">
       <c r="A75">
         <v>74</v>
       </c>
@@ -1585,7 +1746,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:3">
       <c r="A76">
         <v>75</v>
       </c>
@@ -1596,7 +1757,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:3">
       <c r="A77">
         <v>76</v>
       </c>
@@ -1607,7 +1768,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:3">
       <c r="A78">
         <v>77</v>
       </c>
@@ -1618,7 +1779,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:3">
       <c r="A79">
         <v>78</v>
       </c>
@@ -1629,7 +1790,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:3">
       <c r="A80">
         <v>79</v>
       </c>
@@ -1640,7 +1801,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:3">
       <c r="A81">
         <v>80</v>
       </c>
@@ -1658,19 +1819,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A731CCC0-38E9-844C-8737-200721EF57F9}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="2" max="2" width="56.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -1681,103 +1842,48 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="17">
       <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2" s="9">
+        <v>44110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="17">
       <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="C3" s="9">
+        <v>44110</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="17">
       <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="C4" s="9">
+        <v>44110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="17">
       <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" t="s">
-        <v>17</v>
+        <v>29</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C5" s="9">
+        <v>44110</v>
       </c>
     </row>
   </sheetData>
@@ -1787,11 +1893,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E51EBFD-64C4-8C46-8CC8-4B7B052E6AA2}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="3" max="3" width="55.1640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
@@ -1799,7 +1905,7 @@
     <col min="6" max="6" width="52" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -1817,6 +1923,486 @@
       </c>
       <c r="F1" s="2" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E2" t="s">
+        <v>130</v>
+      </c>
+      <c r="F2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3" t="s">
+        <v>129</v>
+      </c>
+      <c r="E3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D4" t="s">
+        <v>129</v>
+      </c>
+      <c r="E4" t="s">
+        <v>131</v>
+      </c>
+      <c r="F4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D5" t="s">
+        <v>129</v>
+      </c>
+      <c r="E5" t="s">
+        <v>131</v>
+      </c>
+      <c r="F5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>133</v>
+      </c>
+      <c r="C6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D6" t="s">
+        <v>134</v>
+      </c>
+      <c r="E6" t="s">
+        <v>131</v>
+      </c>
+      <c r="F6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C7" t="s">
+        <v>107</v>
+      </c>
+      <c r="D7" t="s">
+        <v>129</v>
+      </c>
+      <c r="E7" t="s">
+        <v>131</v>
+      </c>
+      <c r="F7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>133</v>
+      </c>
+      <c r="C8" t="s">
+        <v>105</v>
+      </c>
+      <c r="D8" t="s">
+        <v>134</v>
+      </c>
+      <c r="E8" t="s">
+        <v>131</v>
+      </c>
+      <c r="F8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>135</v>
+      </c>
+      <c r="C9" t="s">
+        <v>107</v>
+      </c>
+      <c r="D9" t="s">
+        <v>129</v>
+      </c>
+      <c r="E9" t="s">
+        <v>131</v>
+      </c>
+      <c r="F9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>135</v>
+      </c>
+      <c r="C10" t="s">
+        <v>107</v>
+      </c>
+      <c r="D10" t="s">
+        <v>129</v>
+      </c>
+      <c r="E10" t="s">
+        <v>131</v>
+      </c>
+      <c r="F10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>135</v>
+      </c>
+      <c r="C11" t="s">
+        <v>107</v>
+      </c>
+      <c r="D11" t="s">
+        <v>129</v>
+      </c>
+      <c r="E11" t="s">
+        <v>131</v>
+      </c>
+      <c r="F11" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>136</v>
+      </c>
+      <c r="C12" t="s">
+        <v>108</v>
+      </c>
+      <c r="D12" t="s">
+        <v>134</v>
+      </c>
+      <c r="E12" t="s">
+        <v>131</v>
+      </c>
+      <c r="F12" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>137</v>
+      </c>
+      <c r="C13" t="s">
+        <v>109</v>
+      </c>
+      <c r="D13" t="s">
+        <v>129</v>
+      </c>
+      <c r="E13" t="s">
+        <v>131</v>
+      </c>
+      <c r="F13" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>138</v>
+      </c>
+      <c r="C14" t="s">
+        <v>110</v>
+      </c>
+      <c r="D14" t="s">
+        <v>134</v>
+      </c>
+      <c r="E14" t="s">
+        <v>131</v>
+      </c>
+      <c r="F14" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>139</v>
+      </c>
+      <c r="C15" t="s">
+        <v>111</v>
+      </c>
+      <c r="D15" t="s">
+        <v>129</v>
+      </c>
+      <c r="E15" t="s">
+        <v>131</v>
+      </c>
+      <c r="F15" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16">
+        <v>17</v>
+      </c>
+      <c r="B16" t="s">
+        <v>140</v>
+      </c>
+      <c r="C16" t="s">
+        <v>113</v>
+      </c>
+      <c r="D16" t="s">
+        <v>129</v>
+      </c>
+      <c r="E16" t="s">
+        <v>131</v>
+      </c>
+      <c r="F16" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17">
+        <v>18</v>
+      </c>
+      <c r="B17" t="s">
+        <v>141</v>
+      </c>
+      <c r="C17" t="s">
+        <v>114</v>
+      </c>
+      <c r="D17" t="s">
+        <v>134</v>
+      </c>
+      <c r="E17" t="s">
+        <v>131</v>
+      </c>
+      <c r="F17" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18">
+        <v>19</v>
+      </c>
+      <c r="B18" t="s">
+        <v>142</v>
+      </c>
+      <c r="C18" t="s">
+        <v>115</v>
+      </c>
+      <c r="D18" t="s">
+        <v>134</v>
+      </c>
+      <c r="E18" t="s">
+        <v>131</v>
+      </c>
+      <c r="F18" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19">
+        <v>21</v>
+      </c>
+      <c r="B19" t="s">
+        <v>143</v>
+      </c>
+      <c r="C19" t="s">
+        <v>117</v>
+      </c>
+      <c r="D19" t="s">
+        <v>134</v>
+      </c>
+      <c r="E19" t="s">
+        <v>131</v>
+      </c>
+      <c r="F19" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20">
+        <v>23</v>
+      </c>
+      <c r="B20" t="s">
+        <v>144</v>
+      </c>
+      <c r="C20" t="s">
+        <v>119</v>
+      </c>
+      <c r="D20" t="s">
+        <v>134</v>
+      </c>
+      <c r="E20" t="s">
+        <v>131</v>
+      </c>
+      <c r="F20" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21">
+        <v>24</v>
+      </c>
+      <c r="B21" t="s">
+        <v>145</v>
+      </c>
+      <c r="C21" t="s">
+        <v>120</v>
+      </c>
+      <c r="D21" t="s">
+        <v>134</v>
+      </c>
+      <c r="E21" t="s">
+        <v>131</v>
+      </c>
+      <c r="F21" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22">
+        <v>25</v>
+      </c>
+      <c r="B22" t="s">
+        <v>146</v>
+      </c>
+      <c r="C22" t="s">
+        <v>121</v>
+      </c>
+      <c r="D22" t="s">
+        <v>129</v>
+      </c>
+      <c r="E22" t="s">
+        <v>131</v>
+      </c>
+      <c r="F22" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23">
+        <v>27</v>
+      </c>
+      <c r="B23" t="s">
+        <v>147</v>
+      </c>
+      <c r="C23" t="s">
+        <v>123</v>
+      </c>
+      <c r="D23" t="s">
+        <v>134</v>
+      </c>
+      <c r="E23" t="s">
+        <v>131</v>
+      </c>
+      <c r="F23" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24">
+        <v>28</v>
+      </c>
+      <c r="B24" t="s">
+        <v>148</v>
+      </c>
+      <c r="C24" t="s">
+        <v>124</v>
+      </c>
+      <c r="D24" t="s">
+        <v>134</v>
+      </c>
+      <c r="E24" t="s">
+        <v>131</v>
+      </c>
+      <c r="F24" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25">
+        <v>29</v>
+      </c>
+      <c r="B25" t="s">
+        <v>149</v>
+      </c>
+      <c r="C25" t="s">
+        <v>125</v>
+      </c>
+      <c r="D25" t="s">
+        <v>134</v>
+      </c>
+      <c r="E25" t="s">
+        <v>131</v>
+      </c>
+      <c r="F25" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -1832,12 +2418,12 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="3" max="3" width="116.5" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -1848,7 +2434,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1859,22 +2445,22 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -1886,43 +2472,335 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A33C8DF8-6616-BA4D-AB61-8CB1886EEA93}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:B46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A22" sqref="A22:B46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="43.1640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1">
       <c r="A3" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1">
       <c r="A4" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1">
       <c r="A5" s="5" t="s">
         <v>15</v>
       </c>
     </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="7" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="17">
+      <c r="A22" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="B22" s="9">
+        <v>44110</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="17">
+      <c r="A23" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B23" s="9">
+        <v>44110</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="17">
+      <c r="A24" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24" s="9">
+        <v>44110</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="17">
+      <c r="A25" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B25" s="9">
+        <v>44110</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="17">
+      <c r="A26" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B26" s="9">
+        <v>44110</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="17">
+      <c r="A27" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="B27" s="9">
+        <v>44110</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="17">
+      <c r="A28" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="B28" s="9">
+        <v>44110</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="17">
+      <c r="A29" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="B29" s="9">
+        <v>44110</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="17">
+      <c r="A30" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B30" s="9">
+        <v>44110</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="17">
+      <c r="A31" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="B31" s="9">
+        <v>44110</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="17">
+      <c r="A32" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B32" s="9">
+        <v>44110</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="17">
+      <c r="A33" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="B33" s="9">
+        <v>44110</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="17">
+      <c r="A34" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="B34" s="9">
+        <v>44110</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="17">
+      <c r="A35" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="B35" s="9">
+        <v>44110</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="17">
+      <c r="A36" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B36" s="9">
+        <v>44110</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="17">
+      <c r="A37" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="B37" s="9">
+        <v>44110</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="17">
+      <c r="A38" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B38" s="9">
+        <v>44110</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="17">
+      <c r="A39" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B39" s="9">
+        <v>44110</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="17">
+      <c r="A40" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B40" s="9">
+        <v>44110</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="17">
+      <c r="A41" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B41" s="9">
+        <v>44110</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="17">
+      <c r="A42" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="B42" s="9">
+        <v>44110</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="17">
+      <c r="A43" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B43" s="9">
+        <v>44110</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="17">
+      <c r="A44" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="B44" s="9">
+        <v>44110</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="17">
+      <c r="A45" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="B45" s="9">
+        <v>44110</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="17">
+      <c r="A46" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="B46" s="9">
+        <v>44110</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A8" r:id="rId1" xr:uid="{7A2BCF8F-7D94-5B4D-99BA-400C77598B99}"/>
+    <hyperlink ref="A9" r:id="rId2" xr:uid="{599995EC-2066-1A44-809D-1209E4B680A5}"/>
+    <hyperlink ref="A10" r:id="rId3" xr:uid="{473FD441-0651-1847-BAA1-B361B704FC88}"/>
+    <hyperlink ref="A11" r:id="rId4" xr:uid="{0487D5FD-FD47-5443-BF82-7C40A981FE02}"/>
+    <hyperlink ref="A12" r:id="rId5" xr:uid="{66A88799-57EE-B54D-9158-6367DC437EB2}"/>
+    <hyperlink ref="A13" r:id="rId6" xr:uid="{93A2E1AE-8649-0F45-A4CF-9BD65DB37E43}"/>
+    <hyperlink ref="A14" r:id="rId7" xr:uid="{08823A76-51E1-F44B-81C7-0444D01FBEDB}"/>
+    <hyperlink ref="A15" r:id="rId8" xr:uid="{E6256009-55EB-1C44-926E-9AA425097124}"/>
+    <hyperlink ref="A16" r:id="rId9" xr:uid="{D1BFEF57-5321-B649-A547-54AF3F4730D9}"/>
+    <hyperlink ref="A21" r:id="rId10" xr:uid="{F73E7507-B36D-3647-AE9C-D71B3B932C1E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -1936,13 +2814,13 @@
       <selection activeCell="C2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="33" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="10.83203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -1956,14 +2834,14 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
-        <v>98</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>